<commit_message>
update sem gse ismt
</commit_message>
<xml_diff>
--- a/3_output/tablas/gse_tables/low_ajust_apbi.xlsx
+++ b/3_output/tablas/gse_tables/low_ajust_apbi.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>5.386278759431661</v>
+        <v>0.5919738843804225</v>
       </c>
     </row>
     <row r="3">
@@ -406,7 +406,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.2941203485620266</v>
+        <v>0.234678462866897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>